<commit_message>
Made final changes and fixes
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reyno\Desktop\Freelancing\bittar_questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E99051-237D-4555-A80F-08FDE22FB90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625D54B1-2B42-4677-9DE1-8DF9A63E365B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5137" yWindow="1320" windowWidth="16200" windowHeight="9308" xr2:uid="{A1ACD433-7779-45E1-B966-D2F452CAC5BA}"/>
+    <workbookView xWindow="3915" yWindow="1740" windowWidth="16200" windowHeight="9308" xr2:uid="{A1ACD433-7779-45E1-B966-D2F452CAC5BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Score (1 to 5)</t>
+  </si>
+  <si>
+    <t>The quick brown fox jumps over the lazy dog, the quick brown fox jumps over the lazy dog</t>
+  </si>
+  <si>
+    <t>Questionnaire 3</t>
+  </si>
+  <si>
+    <t>Text 1</t>
+  </si>
+  <si>
+    <t>Text 2</t>
+  </si>
+  <si>
+    <t>Text 3</t>
+  </si>
+  <si>
+    <t>Text 4</t>
+  </si>
+  <si>
+    <t>Text 5</t>
+  </si>
+  <si>
+    <t>Text 6</t>
+  </si>
+  <si>
+    <t>Text 7</t>
+  </si>
+  <si>
+    <t>Text 8</t>
+  </si>
   <si>
     <t>Questionnaire 1</t>
   </si>
@@ -44,82 +80,25 @@
     <t>Questionnaire 2</t>
   </si>
   <si>
-    <t>Questionnaire 3</t>
-  </si>
-  <si>
-    <t>Item text item text item text item text item text item text item text item text item text item text item text item text item text item text item text.</t>
-  </si>
-  <si>
-    <t>Question text question text question text question text question text question text question text question text</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Score (1 to 5)</t>
-  </si>
-  <si>
-    <t>Scale 1 score</t>
-  </si>
-  <si>
-    <t>Scale 2 score</t>
-  </si>
-  <si>
-    <t>Score ratio</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
-    <t>Result text result text: Ratio = 0</t>
-  </si>
-  <si>
-    <t>Result text result text:: 0.75 ≤ Ratio ≤ 1.25</t>
-  </si>
-  <si>
-    <t>Result text result text: 1.25 &lt; Ratio &lt; 2</t>
-  </si>
-  <si>
-    <t>Result text result text: 0 &lt; Ratio &lt; 0.75</t>
-  </si>
-  <si>
-    <t>Result text result text: Ratio ≥ 2</t>
-  </si>
-  <si>
-    <t>Result text result text: Ratio &gt; 2</t>
-  </si>
-  <si>
-    <t>Result text result text: 1.25 &lt; Ratio ≤ 2</t>
-  </si>
-  <si>
-    <t>Result text result text: 0.5 &lt; Ratio &lt; 0.75</t>
-  </si>
-  <si>
-    <t>Result text result text: Ratio ≤ 0.5</t>
-  </si>
-  <si>
     <t>Final score</t>
   </si>
   <si>
-    <t>1 Item text item text item text item text item text item text item text item text item text item text item text item text item text item text item text.</t>
-  </si>
-  <si>
-    <t>2 Item text item text item text item text item text item text item text item text item text item text item text item text item text item text item text.</t>
-  </si>
-  <si>
-    <t>3 Item text item text item text item text item text item text item text item text item text item text item text item text item text item text item text.</t>
-  </si>
-  <si>
-    <t>4 Item text item text item text item text item text item text item text item text item text item text item text item text item text item text item text.</t>
-  </si>
-  <si>
-    <t>8 Item text item text item text item text item text item text item text item text item text item text item text item text item text item text item text.</t>
-  </si>
-  <si>
-    <t>9 Item text item text item text item text item text item text item text item text item text item text item text item text item text item text item text.</t>
-  </si>
-  <si>
-    <t>16 Item text item text item text item text item text item text item text item text item text item text item text item text item text item text item text.</t>
+    <t>Scale 1 Score</t>
+  </si>
+  <si>
+    <t>Scale 2 Score</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Text text</t>
+  </si>
+  <si>
+    <t>short</t>
   </si>
 </sst>
 </file>
@@ -129,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +133,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Inter"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -548,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F7B809-C9C3-44E3-BCC3-1CBB8601F386}">
   <dimension ref="B1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -557,9 +542,9 @@
     <col min="1" max="1" width="1.3984375" customWidth="1"/>
     <col min="2" max="2" width="177.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.1328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="60.73046875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.1328125" style="1"/>
@@ -568,31 +553,31 @@
     <row r="1" spans="2:9" ht="7.5" customHeight="1"/>
     <row r="2" spans="2:9">
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:9">
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="7">
@@ -609,7 +594,7 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I3" s="9">
         <v>0</v>
@@ -617,7 +602,7 @@
     </row>
     <row r="4" spans="2:9">
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -625,7 +610,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I4" s="9">
         <v>5</v>
@@ -633,7 +618,7 @@
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -641,7 +626,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I5" s="9">
         <v>10</v>
@@ -649,7 +634,7 @@
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -657,7 +642,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I6" s="9">
         <v>20</v>
@@ -665,7 +650,7 @@
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -673,7 +658,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I7" s="9">
         <v>40</v>
@@ -681,7 +666,7 @@
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -691,7 +676,7 @@
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -703,7 +688,7 @@
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -715,7 +700,7 @@
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -727,7 +712,7 @@
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -739,7 +724,7 @@
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -751,7 +736,7 @@
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -763,7 +748,7 @@
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -775,7 +760,7 @@
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -787,7 +772,7 @@
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -799,7 +784,7 @@
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -821,31 +806,31 @@
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="4" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="7">
@@ -862,7 +847,7 @@
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I21" s="9">
         <v>0.5</v>
@@ -870,7 +855,7 @@
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -878,7 +863,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I22" s="9">
         <v>0.625</v>
@@ -886,7 +871,7 @@
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -894,7 +879,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I23" s="9">
         <v>0.75</v>
@@ -902,7 +887,7 @@
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -910,7 +895,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I24" s="9">
         <v>0.875</v>
@@ -918,7 +903,7 @@
     </row>
     <row r="25" spans="2:9">
       <c r="B25" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -934,7 +919,7 @@
     </row>
     <row r="26" spans="2:9">
       <c r="B26" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -946,7 +931,7 @@
     </row>
     <row r="27" spans="2:9">
       <c r="B27" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -958,7 +943,7 @@
     </row>
     <row r="28" spans="2:9">
       <c r="B28" s="4" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -970,7 +955,7 @@
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="4" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -982,7 +967,7 @@
     </row>
     <row r="30" spans="2:9">
       <c r="B30" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -994,7 +979,7 @@
     </row>
     <row r="31" spans="2:9">
       <c r="B31" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1006,7 +991,7 @@
     </row>
     <row r="32" spans="2:9">
       <c r="B32" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1018,7 +1003,7 @@
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1030,7 +1015,7 @@
     </row>
     <row r="34" spans="2:9">
       <c r="B34" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1042,7 +1027,7 @@
     </row>
     <row r="35" spans="2:9">
       <c r="B35" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1054,7 +1039,7 @@
     </row>
     <row r="36" spans="2:9">
       <c r="B36" s="4" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1076,7 +1061,7 @@
     </row>
     <row r="38" spans="2:9">
       <c r="B38" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1085,25 +1070,25 @@
     </row>
     <row r="39" spans="2:9">
       <c r="B39" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="10"/>
       <c r="H39" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="2:9">
       <c r="B40" s="4" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1117,7 +1102,7 @@
     </row>
     <row r="41" spans="2:9">
       <c r="B41" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1131,7 +1116,7 @@
     </row>
     <row r="42" spans="2:9">
       <c r="B42" s="4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1145,7 +1130,7 @@
     </row>
     <row r="43" spans="2:9">
       <c r="B43" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1159,7 +1144,7 @@
     </row>
     <row r="44" spans="2:9">
       <c r="B44" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1173,7 +1158,7 @@
     </row>
     <row r="45" spans="2:9">
       <c r="B45" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1187,7 +1172,7 @@
     </row>
     <row r="46" spans="2:9">
       <c r="B46" s="4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1201,7 +1186,7 @@
     </row>
     <row r="47" spans="2:9">
       <c r="B47" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1263,6 +1248,7 @@
       <c r="H53" s="12"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>